<commit_message>
Release 1.2.0 - statewide validation web site related modifications done.
</commit_message>
<xml_diff>
--- a/src/WpfApp/Assets/modx_sample.xlsx
+++ b/src/WpfApp/Assets/modx_sample.xlsx
@@ -1407,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,8 +1422,9 @@
     <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="64.42578125" customWidth="1"/>
+    <col min="16" max="16" width="46.28515625" customWidth="1"/>
+    <col min="17" max="17" width="66.42578125" customWidth="1"/>
     <col min="18" max="18" width="26" customWidth="1"/>
     <col min="19" max="19" width="28.42578125" customWidth="1"/>
   </cols>

</xml_diff>